<commit_message>
WRI updates to BPMCCS
</commit_message>
<xml_diff>
--- a/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
+++ b/InputData/elec/BPMCCS/BAU Pol Mandated Cap Const Sched.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BPMCCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\BPMCCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3180" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,14 @@
     <sheet name="Calcs" sheetId="3" r:id="rId7"/>
     <sheet name="BPMCCS" sheetId="2" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -213,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="212">
   <si>
     <t>Note:</t>
   </si>
@@ -462,9 +464,6 @@
     <t>case), etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">which have been a significant barrier for tender participation in the RE auctions. </t>
-  </si>
-  <si>
     <t>40% installed capacity is from non-fossil fuels.</t>
   </si>
   <si>
@@ -542,9 +541,6 @@
 achievement (MW)*</t>
   </si>
   <si>
-    <t>* Calculated based on success rate fraction in About tab</t>
-  </si>
-  <si>
     <t>Source: CEA - National Electricity Plan Vol I</t>
   </si>
   <si>
@@ -581,18 +577,6 @@
     <t>Projected RE installed capacity for FY22</t>
   </si>
   <si>
-    <t>News on removal of tariff caps for solar and wind auctions</t>
-  </si>
-  <si>
-    <t>MERCOM India</t>
-  </si>
-  <si>
-    <t>MNRE Mulls Removal of Tariff Caps for Solar and Wind Tenders</t>
-  </si>
-  <si>
-    <t>https://mercomindia.com/mnre-mulls-removal-tariff-caps-solar-wind/</t>
-  </si>
-  <si>
     <t>Classification of large hydro as RE</t>
   </si>
   <si>
@@ -611,37 +595,10 @@
     <t>estimates that only 104 GW would be achieved by 2022 (which is ~60% of the intended target),</t>
   </si>
   <si>
-    <t>due to various hurdles in project commissioning.</t>
-  </si>
-  <si>
-    <t>Further, there is a reclassification of larger hydro as RE recently, which could technically</t>
-  </si>
-  <si>
-    <t>make it possible to reach, or even surpass the 175 GW target by 2022 in terms of a combined</t>
-  </si>
-  <si>
-    <t>and not just by adding large hydro to the mix, which would significantly increase the size of RE.</t>
-  </si>
-  <si>
-    <t>potential removal of tariff caps for wind and solar tenders, it would be possible to reach about</t>
-  </si>
-  <si>
-    <t>80% of the mandated RE target by 2022. The balance capacity remaining, after subtracting the</t>
-  </si>
-  <si>
-    <t>current RE capacities for each source, is divided between 2020 to 2022 for wind and solar.</t>
-  </si>
-  <si>
     <t>For SHP, biomass (and MSW), the targets are already almost reached, and we assume that</t>
   </si>
   <si>
     <t>they will continue to grow at the same rate till 2022 to help reach the 175 GW combined target.</t>
-  </si>
-  <si>
-    <t>The success rate % can be changed in the About tab to accordingly assess the yearly balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacity additions to reach the "adjusted" target. </t>
   </si>
   <si>
     <r>
@@ -699,15 +656,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">we interpret the overall RE target to be achieved on reaching the disaggregated targets, </t>
-  </si>
-  <si>
-    <t>RE target. But since the 175 GW target was disaggregated (for wind, solar, biomass and SHP),</t>
-  </si>
-  <si>
-    <t>Fraction of RE target achievable by 2022</t>
-  </si>
-  <si>
     <t>Capacity Additions 2030 (for calculation only - not used)</t>
   </si>
   <si>
@@ -720,9 +668,6 @@
     <t>http://www.cea.nic.in/reports/monthly/installedcapacity/2017/installed_capacity-12.pdf</t>
   </si>
   <si>
-    <t>In parallel, there are recent reports of potential removal of tariff caps for solar and wind tenders,</t>
-  </si>
-  <si>
     <t xml:space="preserve">In case of 2018 and 2019, actual capacity added is used for the mandated values as actuals are available. </t>
   </si>
   <si>
@@ -793,9 +738,6 @@
   </si>
   <si>
     <t>Planned Capacity Additions till 2022 (RE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We assume in light of recent public announcements of a 450 GW target by 2030, and the </t>
   </si>
   <si>
     <t>Year/MW</t>
@@ -945,6 +887,18 @@
   </si>
   <si>
     <t>http://www.cea.nic.in/reports/monthly/hydro/2019/pump_storage-09.pdf</t>
+  </si>
+  <si>
+    <t>due to various hurdles in project commissioning. We assume this conservative estimate till 2022.</t>
+  </si>
+  <si>
+    <t>* based on CRISIL estimate</t>
+  </si>
+  <si>
+    <t>The balance capacity remaining, after subtracting the current RE capacities</t>
+  </si>
+  <si>
+    <t>from the CRISIL estimate, is apportioned between 2020 to 2022 for wind and solar.</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1486,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1668,6 +1621,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1686,6 +1643,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1695,15 +1661,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1712,9 +1669,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1732,6 +1686,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>25977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3757533</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>110538</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6D40D24-2210-4F41-9C04-B84C529D41E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="701386" y="10122477"/>
+          <a:ext cx="3662283" cy="1989561"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2058,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2080,20 +2083,20 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
-      <c r="B4" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62" t="s">
-        <v>98</v>
+      <c r="B4" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -2102,14 +2105,14 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B6" s="63">
+      <c r="B6" s="62">
         <v>2018</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="62">
         <v>2019</v>
       </c>
     </row>
@@ -2126,23 +2129,23 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B11" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>100</v>
+      <c r="B11" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -2150,14 +2153,14 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="63">
+      <c r="B13" s="62">
         <v>2018</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="62">
         <v>2015</v>
       </c>
     </row>
@@ -2167,7 +2170,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
@@ -2176,7 +2179,7 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
@@ -2185,51 +2188,51 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
-      <c r="B18" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="62" t="s">
-        <v>186</v>
+      <c r="B18" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
-      <c r="B20" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="63"/>
+      <c r="B20" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="62"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -2238,52 +2241,41 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>120</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D25" s="109"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
-      <c r="B26" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>121</v>
-      </c>
+      <c r="B26" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
-      <c r="B28" s="63">
+      <c r="B28" s="62">
         <v>2019</v>
       </c>
-      <c r="D28" s="63">
-        <v>2020</v>
-      </c>
+      <c r="D28" s="62"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -2292,46 +2284,46 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
-      <c r="B33" s="62" t="s">
-        <v>125</v>
+      <c r="B33" s="61" t="s">
+        <v>119</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="130">
+        <v>120</v>
+      </c>
+      <c r="D34" s="108">
         <v>43709</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="2"/>
-      <c r="B35" s="63">
+      <c r="B35" s="62">
         <v>2019</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
       <c r="B36" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -2363,8 +2355,8 @@
       <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" s="108" t="s">
-        <v>224</v>
+      <c r="A44" s="107" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
@@ -2372,12 +2364,12 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
@@ -2385,190 +2377,151 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
-        <v>130</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" s="2" t="s">
-        <v>153</v>
-      </c>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A58" s="2"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="A59" s="2"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" s="2"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" s="2" t="s">
-        <v>178</v>
-      </c>
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" s="73"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A66" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A67" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A68" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A69" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A70" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A72" s="31">
-        <v>0.8</v>
-      </c>
-      <c r="B72" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A73" s="74"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A77" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" s="22" t="s">
-        <v>82</v>
+      <c r="A81" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A84" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A86" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" s="2" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2578,9 +2531,11 @@
     <hyperlink ref="B22" r:id="rId3"/>
     <hyperlink ref="B21" r:id="rId4"/>
     <hyperlink ref="D36" r:id="rId5"/>
+    <hyperlink ref="B29" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2623,27 +2578,27 @@
         <v>831502</v>
       </c>
       <c r="J1" s="6"/>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="78" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
       <c r="G2" s="6"/>
       <c r="H2" s="8" t="s">
         <v>32</v>
@@ -2652,18 +2607,18 @@
         <v>64089</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="80" t="s">
+      <c r="K2" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="81">
+      <c r="L2" s="80">
         <v>47855</v>
       </c>
-      <c r="M2" s="82">
+      <c r="M2" s="81">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="110"/>
+      <c r="A3" s="111"/>
       <c r="B3" s="20" t="s">
         <v>41</v>
       </c>
@@ -2687,13 +2642,13 @@
         <v>5000</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="80" t="s">
+      <c r="K3" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="81">
+      <c r="L3" s="80">
         <v>3300</v>
       </c>
-      <c r="M3" s="82">
+      <c r="M3" s="81">
         <v>6800</v>
       </c>
     </row>
@@ -2724,13 +2679,13 @@
         <v>4356</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="83" t="s">
+      <c r="K4" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="81">
+      <c r="L4" s="80">
         <v>406.15</v>
       </c>
-      <c r="M4" s="82">
+      <c r="M4" s="81">
         <v>0</v>
       </c>
     </row>
@@ -2761,13 +2716,13 @@
         <v>24350</v>
       </c>
       <c r="J5" s="6"/>
-      <c r="K5" s="84" t="s">
+      <c r="K5" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="85">
+      <c r="L5" s="84">
         <v>6822.5</v>
       </c>
-      <c r="M5" s="86">
+      <c r="M5" s="85">
         <v>0</v>
       </c>
     </row>
@@ -2798,11 +2753,11 @@
         <v>266827</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" s="113"/>
-      <c r="M6" s="113"/>
+      <c r="K6" s="113" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
     </row>
     <row r="7" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="16" t="s">
@@ -2868,11 +2823,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
+      <c r="A10" s="113" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
@@ -2889,15 +2844,15 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H12" s="112" t="s">
+      <c r="H12" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="113"/>
+      <c r="I12" s="114"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H13" s="117"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H14" s="14"/>
@@ -2956,12 +2911,12 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="117"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
@@ -2979,7 +2934,7 @@
         <f>I5-C18</f>
         <v>-993.15000000000146</v>
       </c>
-      <c r="H18" s="115"/>
+      <c r="H18" s="116"/>
       <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
@@ -3159,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3179,99 +3134,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A1" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="67"/>
-      <c r="E1" s="69" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="I1" s="69" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="A1" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
+      <c r="E1" s="68" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="I1" s="68" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="36">
+        <v>175</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="33">
+        <f>SUM(F3:F6)</f>
+        <v>119000</v>
+      </c>
+      <c r="G2" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="37">
-        <v>175</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="34">
-        <f>About!A72*'Actuals-based BPMCCS adjustment'!B2*1000</f>
-        <v>140000</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="121"/>
+      <c r="J2" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="126"/>
+      <c r="O2" s="127"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="13">
         <v>100</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <f>B3/175</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="35">
-        <f>C3*$F$2</f>
-        <v>80000</v>
-      </c>
-      <c r="G3" s="38">
+        <v>91</v>
+      </c>
+      <c r="F3" s="34">
+        <v>59000</v>
+      </c>
+      <c r="G3" s="37">
         <f>F3-D12</f>
-        <v>46269.440000000002</v>
-      </c>
-      <c r="I3" s="33" t="s">
+        <v>25269.440000000002</v>
+      </c>
+      <c r="I3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="44" t="s">
+      <c r="O3" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="O3" s="45" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
@@ -3281,7 +3235,7 @@
       <c r="B4" s="13">
         <v>60</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <f>B4/175</f>
         <v>0.34285714285714286</v>
       </c>
@@ -3289,13 +3243,12 @@
       <c r="E4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="36">
-        <f>C4*$F$2</f>
-        <v>48000</v>
-      </c>
-      <c r="G4" s="38">
+      <c r="F4" s="35">
+        <v>45000</v>
+      </c>
+      <c r="G4" s="37">
         <f>F4-D13</f>
-        <v>10494.82</v>
+        <v>7494.82</v>
       </c>
       <c r="I4" s="13">
         <v>2017</v>
@@ -3321,24 +3274,24 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="30">
         <v>5</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <f>B5/175</f>
         <v>2.8571428571428571E-2</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="36">
+        <v>86</v>
+      </c>
+      <c r="F5" s="35">
         <f>B5*1000</f>
         <v>5000</v>
       </c>
-      <c r="G5" s="40"/>
+      <c r="G5" s="39"/>
       <c r="I5" s="13">
         <v>2018</v>
       </c>
@@ -3368,7 +3321,7 @@
       <c r="B6" s="30">
         <v>10</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <f>B6/175</f>
         <v>5.7142857142857141E-2</v>
       </c>
@@ -3376,11 +3329,11 @@
       <c r="E6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <f>B6*1000</f>
         <v>10000</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="40"/>
       <c r="I6" s="13">
         <v>2019</v>
       </c>
@@ -3404,59 +3357,59 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A7" s="46" t="s">
-        <v>105</v>
+      <c r="A7" s="45" t="s">
+        <v>104</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="46" t="s">
-        <v>107</v>
+      <c r="E7" s="45" t="s">
+        <v>209</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="I7" s="46" t="s">
-        <v>158</v>
+      <c r="I7" s="45" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A8" s="46"/>
+      <c r="A8" s="45"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="46"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A9" s="71" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="A9" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="111" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="122"/>
+      <c r="B10" s="112" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="121"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="R10" s="28"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A11" s="110"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="20">
         <v>2017</v>
       </c>
@@ -3493,20 +3446,20 @@
         <f>O6</f>
         <v>33730.559999999998</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="46">
         <f>D12+$G$3/3</f>
-        <v>49153.706666666665</v>
-      </c>
-      <c r="F12" s="47">
+        <v>42153.706666666665</v>
+      </c>
+      <c r="F12" s="46">
         <f>E12+$G$3/3</f>
-        <v>64576.853333333333</v>
-      </c>
-      <c r="G12" s="48">
+        <v>50576.853333333333</v>
+      </c>
+      <c r="G12" s="47">
         <f>F12+$G$3/3</f>
-        <v>80000</v>
+        <v>59000</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I12" s="24"/>
     </row>
@@ -3526,20 +3479,20 @@
         <f>L6</f>
         <v>37505.18</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E13" s="48">
         <f>D13+$G$4/3</f>
-        <v>41003.453333333331</v>
-      </c>
-      <c r="F13" s="49">
+        <v>40003.453333333331</v>
+      </c>
+      <c r="F13" s="48">
         <f>E13+$G$4/3</f>
-        <v>44501.726666666662</v>
-      </c>
-      <c r="G13" s="50">
+        <v>42501.726666666662</v>
+      </c>
+      <c r="G13" s="49">
         <f>F13+$G$4/3</f>
-        <v>47999.999999999993</v>
+        <v>44999.999999999993</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -3558,25 +3511,25 @@
         <f>M6</f>
         <v>9861.31</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="48">
         <f>TREND($C$14:$D$14,$C$11:$D$11,E11)</f>
         <v>10647.120000000112</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="48">
         <f>TREND($C$14:$D$14,$C$11:$D$11,F11)</f>
         <v>11432.930000000168</v>
       </c>
-      <c r="G14" s="50">
+      <c r="G14" s="49">
         <f>TREND($C$14:$D$14,$C$11:$D$11,G11)</f>
         <v>12218.739999999991</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="29">
         <f>K4</f>
@@ -3590,25 +3543,25 @@
         <f>K6</f>
         <v>4671.5600000000004</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="48">
         <f>TREND($C$15:$D$15,$C$11:$D$11,E11)</f>
         <v>4825.6699999999837</v>
       </c>
-      <c r="F15" s="49">
+      <c r="F15" s="48">
         <f>TREND($C$15:$D$15,$C$11:$D$11,F11)</f>
         <v>4979.7799999999697</v>
       </c>
-      <c r="G15" s="50">
+      <c r="G15" s="49">
         <f>TREND($C$15:$D$15,$C$11:$D$11,G11)</f>
         <v>5133.8899999999558</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="29">
         <f>N4</f>
@@ -3622,125 +3575,125 @@
         <f>N6</f>
         <v>139.80000000000001</v>
       </c>
-      <c r="E16" s="51">
+      <c r="E16" s="50">
         <f>TREND($C$16:$D$16,$C$11:$D$11,E11)</f>
         <v>141.30000000000018</v>
       </c>
-      <c r="F16" s="51">
+      <c r="F16" s="50">
         <f>TREND($C$16:$D$16,$C$11:$D$11,F11)</f>
         <v>142.80000000000018</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G16" s="51">
         <f>TREND($C$16:$D$16,$C$11:$D$11,G11)</f>
         <v>144.30000000000018</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A18" s="69" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="I18" s="69" t="s">
-        <v>180</v>
-      </c>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
+      <c r="A18" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="I18" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="111" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="111"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="H19" s="76"/>
-      <c r="J19" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="K19" s="120"/>
-      <c r="L19" s="120"/>
-      <c r="M19" s="120"/>
-      <c r="N19" s="120"/>
-      <c r="O19" s="121"/>
+      <c r="B19" s="112" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="H19" s="75"/>
+      <c r="J19" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="126"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="126"/>
+      <c r="N19" s="126"/>
+      <c r="O19" s="127"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A20" s="110"/>
-      <c r="B20" s="53">
+      <c r="A20" s="111"/>
+      <c r="B20" s="52">
         <v>2018</v>
       </c>
-      <c r="C20" s="53">
+      <c r="C20" s="52">
         <v>2019</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="52">
         <v>2020</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="52">
         <v>2021</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="53">
         <v>2022</v>
       </c>
       <c r="H20" s="24"/>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="L20" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="O20" s="44" t="s">
         <v>161</v>
-      </c>
-      <c r="K20" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="L20" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="N20" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="O20" s="45" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="87">
+      <c r="B21" s="86">
         <f>C12-B12</f>
         <v>8159.8499999999985</v>
       </c>
-      <c r="C21" s="87">
+      <c r="C21" s="86">
         <f>D12-C12</f>
         <v>8518.2999999999993</v>
       </c>
-      <c r="D21" s="55">
+      <c r="D21" s="54">
         <f>E12-D12</f>
-        <v>15423.146666666667</v>
-      </c>
-      <c r="E21" s="55">
+        <v>8423.1466666666674</v>
+      </c>
+      <c r="E21" s="54">
         <f>F12-E12</f>
-        <v>15423.146666666667</v>
-      </c>
-      <c r="F21" s="56">
+        <v>8423.1466666666674</v>
+      </c>
+      <c r="F21" s="55">
         <f>G12-F12</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="13">
@@ -3769,27 +3722,27 @@
       <c r="A22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="88">
+      <c r="B22" s="87">
         <f t="shared" ref="B22:F22" si="0">C13-B13</f>
         <v>2289.6900000000023</v>
       </c>
-      <c r="C22" s="88">
+      <c r="C22" s="87">
         <f t="shared" si="0"/>
         <v>2367.0299999999988</v>
       </c>
-      <c r="D22" s="57">
+      <c r="D22" s="56">
         <f t="shared" si="0"/>
-        <v>3498.2733333333308</v>
-      </c>
-      <c r="E22" s="57">
+        <v>2498.2733333333308</v>
+      </c>
+      <c r="E22" s="56">
         <f t="shared" si="0"/>
-        <v>3498.2733333333308</v>
-      </c>
-      <c r="F22" s="58">
+        <v>2498.2733333333308</v>
+      </c>
+      <c r="F22" s="57">
         <f t="shared" si="0"/>
-        <v>3498.2733333333308</v>
-      </c>
-      <c r="H22" s="42"/>
+        <v>2498.2733333333308</v>
+      </c>
+      <c r="H22" s="41"/>
       <c r="I22" s="13">
         <v>2018</v>
       </c>
@@ -3816,23 +3769,23 @@
       <c r="A23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="88">
+      <c r="B23" s="87">
         <f t="shared" ref="B23" si="1">C14-B14</f>
         <v>661.70000000000073</v>
       </c>
-      <c r="C23" s="88">
+      <c r="C23" s="87">
         <f t="shared" ref="C23:F25" si="2">D14-C14</f>
         <v>785.80999999999949</v>
       </c>
-      <c r="D23" s="57">
+      <c r="D23" s="56">
         <f t="shared" si="2"/>
         <v>785.81000000011227</v>
       </c>
-      <c r="E23" s="57">
+      <c r="E23" s="56">
         <f t="shared" si="2"/>
         <v>785.81000000005588</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="57">
         <f t="shared" si="2"/>
         <v>785.80999999982305</v>
       </c>
@@ -3861,115 +3814,115 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="88">
+        <v>86</v>
+      </c>
+      <c r="B24" s="87">
         <f>C15-B15</f>
         <v>99.300000000000182</v>
       </c>
-      <c r="C24" s="88">
+      <c r="C24" s="87">
         <f t="shared" si="2"/>
         <v>154.11000000000058</v>
       </c>
-      <c r="D24" s="57">
+      <c r="D24" s="56">
         <f t="shared" si="2"/>
         <v>154.1099999999833</v>
       </c>
-      <c r="E24" s="57">
+      <c r="E24" s="56">
         <f t="shared" si="2"/>
         <v>154.10999999998603</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="57">
         <f t="shared" si="2"/>
         <v>154.10999999998603</v>
       </c>
-      <c r="I24" s="46" t="s">
-        <v>158</v>
+      <c r="I24" s="45" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="89">
+        <v>87</v>
+      </c>
+      <c r="B25" s="88">
         <f>C16-B16</f>
         <v>24.220000000000013</v>
       </c>
-      <c r="C25" s="89">
+      <c r="C25" s="88">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="58">
         <f t="shared" si="2"/>
         <v>1.5000000000001705</v>
       </c>
-      <c r="E25" s="59">
+      <c r="E25" s="58">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="F25" s="60">
+      <c r="F25" s="59">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="28" spans="1:18" ht="26.65" x14ac:dyDescent="0.45">
-      <c r="A28" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
+      <c r="A28" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="69"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
       <c r="H28" s="12"/>
-      <c r="J28" s="101" t="s">
+      <c r="J28" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="91" t="s">
+      <c r="K28" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="92" t="s">
+      <c r="L28" s="91" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="123" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="111"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="122"/>
+      <c r="B29" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="112"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="121"/>
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
-      <c r="J29" s="93" t="s">
+      <c r="J29" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="94">
+      <c r="K29" s="93">
         <v>47855</v>
       </c>
-      <c r="L29" s="95">
+      <c r="L29" s="94">
         <v>0</v>
       </c>
       <c r="R29" s="28"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A30" s="110"/>
-      <c r="B30" s="100">
+      <c r="A30" s="111"/>
+      <c r="B30" s="99">
         <v>2017</v>
       </c>
       <c r="C30" s="20">
@@ -3988,19 +3941,19 @@
         <v>2022</v>
       </c>
       <c r="I30" s="11"/>
-      <c r="J30" s="93" t="s">
+      <c r="J30" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="94">
+      <c r="K30" s="93">
         <v>3300</v>
       </c>
-      <c r="L30" s="95">
+      <c r="L30" s="94">
         <v>6800</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B31" s="29">
         <f>J21</f>
@@ -4014,35 +3967,35 @@
         <f>J23</f>
         <v>198494.5</v>
       </c>
-      <c r="E31" s="48">
+      <c r="E31" s="47">
         <f>D31+$K$29/5</f>
         <v>208065.5</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="47">
         <f>E31+$K$29/5</f>
         <v>217636.5</v>
       </c>
-      <c r="G31" s="48">
+      <c r="G31" s="47">
         <f>F31+$K$29/5</f>
         <v>227207.5</v>
       </c>
       <c r="H31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="96" t="s">
+      <c r="J31" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="K31" s="94">
+      <c r="K31" s="93">
         <v>406.15</v>
       </c>
-      <c r="L31" s="95">
+      <c r="L31" s="94">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="16" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B32" s="29">
         <f>K21-B36</f>
@@ -4056,28 +4009,28 @@
         <f>K23-D36</f>
         <v>24587.22</v>
       </c>
-      <c r="E32" s="50">
+      <c r="E32" s="49">
         <f>D32+$K$31/5</f>
         <v>24668.45</v>
       </c>
-      <c r="F32" s="50">
+      <c r="F32" s="49">
         <f>E32+$K$31/5</f>
         <v>24749.68</v>
       </c>
-      <c r="G32" s="50">
+      <c r="G32" s="49">
         <f>F32+$K$31/5</f>
         <v>24830.91</v>
       </c>
       <c r="H32" t="s">
-        <v>94</v>
-      </c>
-      <c r="J32" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="K32" s="98">
+      <c r="K32" s="97">
         <v>6822.5</v>
       </c>
-      <c r="L32" s="99">
+      <c r="L32" s="98">
         <v>0</v>
       </c>
     </row>
@@ -4097,26 +4050,26 @@
         <f>L23</f>
         <v>6780</v>
       </c>
-      <c r="E33" s="50">
+      <c r="E33" s="49">
         <f>D33+$K$30/5</f>
         <v>7440</v>
       </c>
-      <c r="F33" s="50">
+      <c r="F33" s="49">
         <f>E33+$K$30/5</f>
         <v>8100</v>
       </c>
-      <c r="G33" s="50">
+      <c r="G33" s="49">
         <f>F33+$K$30/5</f>
         <v>8760</v>
       </c>
       <c r="H33" t="s">
-        <v>94</v>
-      </c>
-      <c r="J33" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="K33" s="113"/>
-      <c r="L33" s="113"/>
+        <v>93</v>
+      </c>
+      <c r="J33" s="113" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="114"/>
+      <c r="L33" s="114"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
@@ -4134,20 +4087,20 @@
         <f>M23</f>
         <v>45399.22</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="49">
         <f>D34+$K$32/5</f>
         <v>46763.72</v>
       </c>
-      <c r="F34" s="50">
+      <c r="F34" s="49">
         <f>E34+$K$32/5</f>
         <v>48128.22</v>
       </c>
-      <c r="G34" s="50">
+      <c r="G34" s="49">
         <f>F34+$K$32/5</f>
         <v>49492.72</v>
       </c>
       <c r="H34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
@@ -4166,22 +4119,22 @@
         <f>N23</f>
         <v>6760</v>
       </c>
-      <c r="E35" s="50">
-        <v>0</v>
-      </c>
-      <c r="F35" s="50">
-        <v>0</v>
-      </c>
-      <c r="G35" s="50">
+      <c r="E35" s="49">
+        <v>0</v>
+      </c>
+      <c r="F35" s="49">
+        <v>0</v>
+      </c>
+      <c r="G35" s="49">
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B36" s="29">
         <f>B51</f>
@@ -4195,22 +4148,22 @@
         <f>B51</f>
         <v>350</v>
       </c>
-      <c r="E36" s="50">
-        <v>0</v>
-      </c>
-      <c r="F36" s="50">
-        <v>0</v>
-      </c>
-      <c r="G36" s="50">
+      <c r="E36" s="49">
+        <v>0</v>
+      </c>
+      <c r="F36" s="49">
+        <v>0</v>
+      </c>
+      <c r="G36" s="49">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B37" s="29">
         <f>O21</f>
@@ -4224,167 +4177,167 @@
         <f>O23</f>
         <v>509.71</v>
       </c>
-      <c r="E37" s="52">
-        <v>0</v>
-      </c>
-      <c r="F37" s="52">
-        <v>0</v>
-      </c>
-      <c r="G37" s="52">
+      <c r="E37" s="51">
+        <v>0</v>
+      </c>
+      <c r="F37" s="51">
+        <v>0</v>
+      </c>
+      <c r="G37" s="51">
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A39" s="69" t="s">
-        <v>163</v>
-      </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
+      <c r="A39" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A40" s="109" t="s">
+      <c r="A40" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="124" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" s="124"/>
-      <c r="D40" s="124"/>
-      <c r="E40" s="124"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="125"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="125"/>
-      <c r="K40" s="126"/>
+      <c r="B40" s="122" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="122"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
+      <c r="I40" s="123"/>
+      <c r="J40" s="123"/>
+      <c r="K40" s="124"/>
       <c r="M40" s="28"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A41" s="110"/>
-      <c r="B41" s="54">
+      <c r="A41" s="111"/>
+      <c r="B41" s="53">
         <v>2018</v>
       </c>
-      <c r="C41" s="53">
+      <c r="C41" s="52">
         <v>2019</v>
       </c>
-      <c r="D41" s="53">
+      <c r="D41" s="52">
         <v>2020</v>
       </c>
-      <c r="E41" s="53">
+      <c r="E41" s="52">
         <v>2021</v>
       </c>
-      <c r="F41" s="54">
+      <c r="F41" s="53">
         <v>2022</v>
       </c>
-      <c r="G41" s="53">
+      <c r="G41" s="52">
         <v>2023</v>
       </c>
-      <c r="H41" s="53">
+      <c r="H41" s="52">
         <v>2024</v>
       </c>
-      <c r="I41" s="53">
+      <c r="I41" s="52">
         <v>2025</v>
       </c>
-      <c r="J41" s="53">
+      <c r="J41" s="52">
         <v>2026</v>
       </c>
-      <c r="K41" s="54">
+      <c r="K41" s="53">
         <v>2027</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B42" s="87">
+        <v>142</v>
+      </c>
+      <c r="B42" s="86">
         <f>C31-(B31-'BCRbQ Data'!B2)</f>
         <v>110</v>
       </c>
-      <c r="C42" s="87">
+      <c r="C42" s="86">
         <f>D31-(C31-'BCRbQ Data'!C2)</f>
         <v>8697</v>
       </c>
-      <c r="D42" s="55">
+      <c r="D42" s="54">
         <f>E31-D31</f>
         <v>9571</v>
       </c>
-      <c r="E42" s="55">
+      <c r="E42" s="54">
         <f>F31-E31</f>
         <v>9571</v>
       </c>
-      <c r="F42" s="55">
+      <c r="F42" s="54">
         <f t="shared" ref="F42" si="3">G31-F31</f>
         <v>9571</v>
       </c>
-      <c r="G42" s="55">
+      <c r="G42" s="54">
         <f>$L$29/5</f>
         <v>0</v>
       </c>
-      <c r="H42" s="55">
+      <c r="H42" s="54">
         <f t="shared" ref="H42:K42" si="4">$L$29/5</f>
         <v>0</v>
       </c>
-      <c r="I42" s="55">
+      <c r="I42" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J42" s="55">
+      <c r="J42" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K42" s="55">
+      <c r="K42" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" s="88">
+        <v>147</v>
+      </c>
+      <c r="B43" s="87">
         <f>IF((C32-(B32-'BCRbQ Data'!B3))&lt;=0,1,C32-(B32-'BCRbQ Data'!B3))</f>
         <v>1</v>
       </c>
-      <c r="C43" s="88">
+      <c r="C43" s="87">
         <f t="shared" ref="B43:C47" si="5">IF((D32-C32)&lt;=0,1,D32-C32)</f>
         <v>1</v>
       </c>
-      <c r="D43" s="57">
+      <c r="D43" s="56">
         <f t="shared" ref="D43:F45" si="6">E32-D32</f>
         <v>81.229999999999563</v>
       </c>
-      <c r="E43" s="57">
+      <c r="E43" s="56">
         <f t="shared" si="6"/>
         <v>81.229999999999563</v>
       </c>
-      <c r="F43" s="57">
+      <c r="F43" s="56">
         <f t="shared" si="6"/>
         <v>81.229999999999563</v>
       </c>
-      <c r="G43" s="57">
+      <c r="G43" s="56">
         <f>$L$31/5</f>
         <v>0</v>
       </c>
-      <c r="H43" s="57">
+      <c r="H43" s="56">
         <f t="shared" ref="H43:K43" si="7">$L$31/5</f>
         <v>0</v>
       </c>
-      <c r="I43" s="57">
+      <c r="I43" s="56">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J43" s="57">
+      <c r="J43" s="56">
         <f>$L$31/5</f>
         <v>0</v>
       </c>
-      <c r="K43" s="57">
+      <c r="K43" s="56">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4395,43 +4348,43 @@
       <c r="A44" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="88">
+      <c r="B44" s="87">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="C44" s="88">
+      <c r="C44" s="87">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="D44" s="57">
+      <c r="D44" s="56">
         <f t="shared" si="6"/>
         <v>660</v>
       </c>
-      <c r="E44" s="57">
+      <c r="E44" s="56">
         <f t="shared" si="6"/>
         <v>660</v>
       </c>
-      <c r="F44" s="57">
+      <c r="F44" s="56">
         <f t="shared" si="6"/>
         <v>660</v>
       </c>
-      <c r="G44" s="57">
+      <c r="G44" s="56">
         <f>$L$30/5</f>
         <v>1360</v>
       </c>
-      <c r="H44" s="57">
+      <c r="H44" s="56">
         <f t="shared" ref="H44:K44" si="8">$L$30/5</f>
         <v>1360</v>
       </c>
-      <c r="I44" s="57">
+      <c r="I44" s="56">
         <f t="shared" si="8"/>
         <v>1360</v>
       </c>
-      <c r="J44" s="57">
+      <c r="J44" s="56">
         <f t="shared" si="8"/>
         <v>1360</v>
       </c>
-      <c r="K44" s="57">
+      <c r="K44" s="56">
         <f t="shared" si="8"/>
         <v>1360</v>
       </c>
@@ -4441,43 +4394,43 @@
       <c r="A45" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="88">
+      <c r="B45" s="87">
         <f t="shared" si="5"/>
         <v>435.80000000000291</v>
       </c>
-      <c r="C45" s="88">
+      <c r="C45" s="87">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="D45" s="57">
+      <c r="D45" s="56">
         <f t="shared" si="6"/>
         <v>1364.5</v>
       </c>
-      <c r="E45" s="57">
+      <c r="E45" s="56">
         <f t="shared" si="6"/>
         <v>1364.5</v>
       </c>
-      <c r="F45" s="57">
+      <c r="F45" s="56">
         <f t="shared" si="6"/>
         <v>1364.5</v>
       </c>
-      <c r="G45" s="57">
+      <c r="G45" s="56">
         <f>$L$32/5</f>
         <v>0</v>
       </c>
-      <c r="H45" s="57">
+      <c r="H45" s="56">
         <f t="shared" ref="H45:K45" si="9">$L$32/5</f>
         <v>0</v>
       </c>
-      <c r="I45" s="57">
+      <c r="I45" s="56">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J45" s="57">
+      <c r="J45" s="56">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K45" s="57">
+      <c r="K45" s="56">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4486,88 +4439,88 @@
       <c r="A46" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="88">
+      <c r="B46" s="87">
         <f>C35-(B35-'BCRbQ Data'!B13)</f>
         <v>6360</v>
       </c>
-      <c r="C46" s="88">
+      <c r="C46" s="87">
         <f>D35-(C35-'BCRbQ Data'!C13)</f>
         <v>500</v>
       </c>
-      <c r="D46" s="57">
+      <c r="D46" s="56">
         <f>MAX(0,E35-D35)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="57">
+      <c r="E46" s="56">
         <f t="shared" ref="E46:F48" si="10">F35-E35</f>
         <v>0</v>
       </c>
-      <c r="F46" s="57">
+      <c r="F46" s="56">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G46" s="57">
+      <c r="G46" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H46" s="57">
+      <c r="H46" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I46" s="57">
+      <c r="I46" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="J46" s="57">
+      <c r="J46" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K46" s="57">
+      <c r="K46" s="56">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B47" s="88">
+        <v>148</v>
+      </c>
+      <c r="B47" s="87">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="C47" s="88">
+      <c r="C47" s="87">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="D47" s="57">
+      <c r="D47" s="56">
         <f>MAX(0,E36-D36)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="57">
+      <c r="E47" s="56">
         <f>F36-E36</f>
         <v>0</v>
       </c>
-      <c r="F47" s="57">
+      <c r="F47" s="56">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G47" s="57">
+      <c r="G47" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H47" s="57">
+      <c r="H47" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I47" s="57">
+      <c r="I47" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="J47" s="57">
+      <c r="J47" s="56">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="K47" s="57">
+      <c r="K47" s="56">
         <f>0</f>
         <v>0</v>
       </c>
@@ -4576,45 +4529,45 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B48" s="89">
+        <v>161</v>
+      </c>
+      <c r="B48" s="88">
         <f>IF((C37-(B37-'BCRbQ Data'!B11))&lt;=0,1,C37-(B37-'BCRbQ Data'!B11))</f>
         <v>1</v>
       </c>
-      <c r="C48" s="89">
+      <c r="C48" s="88">
         <f>IF((D37-(C37-'BCRbQ Data'!C11))&lt;=0,1,D37-(C37-'BCRbQ Data'!C11))</f>
         <v>1</v>
       </c>
-      <c r="D48" s="59">
+      <c r="D48" s="58">
         <f>MAX(0,E37-D37)</f>
         <v>0</v>
       </c>
-      <c r="E48" s="59">
+      <c r="E48" s="58">
         <f>F37-E37</f>
         <v>0</v>
       </c>
-      <c r="F48" s="59">
+      <c r="F48" s="58">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G48" s="59">
+      <c r="G48" s="58">
         <f>F48</f>
         <v>0</v>
       </c>
-      <c r="H48" s="59">
+      <c r="H48" s="58">
         <f t="shared" ref="H48:J48" si="11">G48</f>
         <v>0</v>
       </c>
-      <c r="I48" s="59">
+      <c r="I48" s="58">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J48" s="59">
+      <c r="J48" s="58">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K48" s="59">
+      <c r="K48" s="58">
         <f>J48</f>
         <v>0</v>
       </c>
@@ -4625,44 +4578,44 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" s="90" t="s">
-        <v>164</v>
+      <c r="A51" s="89" t="s">
+        <v>145</v>
       </c>
       <c r="B51">
         <v>350</v>
       </c>
       <c r="C51" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B40:K40"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="J19:O19"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B40:K40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4687,14 +4640,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="127" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="128"/>
+      <c r="G1" s="128" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="129"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B2" s="1">
         <v>2017</v>
@@ -5125,7 +5078,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -5192,7 +5145,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5328,49 +5281,49 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="102" t="s">
-        <v>191</v>
+      <c r="A1" s="101" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="102" t="s">
-        <v>192</v>
+      <c r="A2" s="101" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="102" t="s">
-        <v>193</v>
+      <c r="A3" s="101" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="103"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="129" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="129"/>
+      <c r="C4" s="130" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="130"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="104" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="104" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="105" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>198</v>
+      <c r="A5" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="103" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="104" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A6" s="106" t="s">
-        <v>199</v>
+      <c r="A6" s="105" t="s">
+        <v>179</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -5378,8 +5331,8 @@
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="106" t="s">
-        <v>200</v>
+      <c r="A7" s="105" t="s">
+        <v>180</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -5391,10 +5344,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="D8" s="16">
         <v>705.6</v>
@@ -5406,10 +5359,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="D9" s="13">
         <v>400</v>
@@ -5421,10 +5374,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="D10" s="13">
         <v>150</v>
@@ -5436,10 +5389,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="D11" s="13">
         <v>900</v>
@@ -5451,10 +5404,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="D12" s="13">
         <v>900</v>
@@ -5466,10 +5419,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D13" s="13">
         <v>250</v>
@@ -5477,10 +5430,10 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="106"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="D14" s="13">
         <f>SUM(D8:D13)</f>
@@ -5496,8 +5449,8 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A16" s="106" t="s">
-        <v>214</v>
+      <c r="A16" s="105" t="s">
+        <v>194</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -5509,16 +5462,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="D17" s="13">
         <v>1000</v>
       </c>
-      <c r="E17" s="107" t="s">
-        <v>217</v>
+      <c r="E17" s="106" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.45">
@@ -5526,16 +5479,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="D18" s="13">
         <v>80</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.45">
@@ -5543,16 +5496,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="D19" s="13">
         <v>500</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.45">
@@ -5667,7 +5620,7 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="B22" s="28">
         <f>D22</f>
@@ -6005,7 +5958,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="74" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="15">
@@ -6018,19 +5971,19 @@
       </c>
       <c r="D6" s="15">
         <f>'Actuals-based BPMCCS adjustment'!D22</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
       <c r="E6" s="15">
         <f>'Actuals-based BPMCCS adjustment'!E22</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
       <c r="F6" s="15">
         <f>'Actuals-based BPMCCS adjustment'!F22</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="74" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="15">
@@ -6043,24 +5996,24 @@
       </c>
       <c r="D7" s="15">
         <f>'Actuals-based BPMCCS adjustment'!D21</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="E7" s="15">
         <f>'Actuals-based BPMCCS adjustment'!E21</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="F7" s="15">
         <f>'Actuals-based BPMCCS adjustment'!F21</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="74" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="28">
@@ -6164,7 +6117,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="74" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="28">
@@ -6200,8 +6153,8 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6829,15 +6782,15 @@
       </c>
       <c r="G6" s="28">
         <f>Calcs!D6</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
       <c r="H6" s="28">
         <f>Calcs!E6</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
       <c r="I6" s="28">
         <f>Calcs!F6</f>
-        <v>3498.2733333333308</v>
+        <v>2498.2733333333308</v>
       </c>
       <c r="J6" s="28">
         <f>Calcs!G6</f>
@@ -6948,15 +6901,15 @@
       </c>
       <c r="G7" s="28">
         <f>Calcs!D7</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="H7" s="28">
         <f>Calcs!E7</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="I7" s="28">
         <f>Calcs!F7</f>
-        <v>15423.146666666667</v>
+        <v>8423.1466666666674</v>
       </c>
       <c r="J7" s="28">
         <f>Calcs!G7</f>

</xml_diff>